<commit_message>
Fixes & added callback function to update state of main app once a user is found
</commit_message>
<xml_diff>
--- a/data/Crunch Schema.xlsx
+++ b/data/Crunch Schema.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mattelacqua/Workspace/crunch/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88A4290A-BEB2-6D41-A72B-88745706A79D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA7C0ACD-3A3F-D848-85E1-93F99DCEE223}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="800" yWindow="4540" windowWidth="29340" windowHeight="21720" xr2:uid="{92CC6430-EF71-6B47-B59B-C2C0DA22E43B}"/>
+    <workbookView xWindow="-29980" yWindow="760" windowWidth="29340" windowHeight="18880" xr2:uid="{92CC6430-EF71-6B47-B59B-C2C0DA22E43B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="57">
   <si>
     <t xml:space="preserve">USER </t>
   </si>
@@ -140,9 +140,6 @@
   </si>
   <si>
     <t>twitter</t>
-  </si>
-  <si>
-    <t>curr_employer</t>
   </si>
   <si>
     <t>street</t>
@@ -581,8 +578,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AFE5892-959D-F94B-B9B4-46E79E09F75E}">
   <dimension ref="A1:Q18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3:M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -666,9 +663,7 @@
       <c r="K3" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="L3" s="1" t="s">
-        <v>35</v>
-      </c>
+      <c r="L3" s="1"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="2"/>
@@ -843,49 +838,49 @@
         <v>26</v>
       </c>
       <c r="C15" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E15" s="1" t="s">
+      <c r="F15" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="G15" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="G15" s="1" t="s">
+      <c r="H15" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="H15" s="1" t="s">
+      <c r="I15" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="I15" s="1" t="s">
+      <c r="J15" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="J15" s="1" t="s">
+      <c r="K15" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="K15" s="1" t="s">
+      <c r="L15" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="L15" s="1" t="s">
+      <c r="M15" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="M15" s="1" t="s">
+      <c r="N15" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="N15" s="1" t="s">
+      <c r="O15" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="O15" s="1" t="s">
+      <c r="P15" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="P15" s="1" t="s">
-        <v>56</v>
-      </c>
       <c r="Q15" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.2">
@@ -943,25 +938,25 @@
         <v>26</v>
       </c>
       <c r="C18" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D18" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E18" s="1" t="s">
+      <c r="F18" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="G18" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="G18" s="1" t="s">
+      <c r="H18" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H18" s="1" t="s">
+      <c r="I18" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="I18" s="1" t="s">
-        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added the csv reading for applications spreadsheet util. Need to add backend database integrations with it. Should probably refresh the db with whatever you import as the CSV.
</commit_message>
<xml_diff>
--- a/data/Crunch Schema.xlsx
+++ b/data/Crunch Schema.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mattelacqua/Workspace/crunch/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA7C0ACD-3A3F-D848-85E1-93F99DCEE223}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E71746E-05F1-3F41-8A78-32C6CF5B0D77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-29980" yWindow="760" windowWidth="29340" windowHeight="18880" xr2:uid="{92CC6430-EF71-6B47-B59B-C2C0DA22E43B}"/>
+    <workbookView xWindow="-28300" yWindow="760" windowWidth="26700" windowHeight="17700" xr2:uid="{92CC6430-EF71-6B47-B59B-C2C0DA22E43B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="56">
   <si>
     <t xml:space="preserve">USER </t>
   </si>
@@ -43,9 +42,6 @@
     <t>Name</t>
   </si>
   <si>
-    <t>ID</t>
-  </si>
-  <si>
     <t>Education</t>
   </si>
   <si>
@@ -94,15 +90,9 @@
     <t>Job Title</t>
   </si>
   <si>
-    <t>Location</t>
-  </si>
-  <si>
     <t>Company</t>
   </si>
   <si>
-    <t>Description</t>
-  </si>
-  <si>
     <t>TEXT</t>
   </si>
   <si>
@@ -163,9 +153,6 @@
     <t>street2</t>
   </si>
   <si>
-    <t>directory</t>
-  </si>
-  <si>
     <t>code</t>
   </si>
   <si>
@@ -178,24 +165,9 @@
     <t>remote</t>
   </si>
   <si>
-    <t>status</t>
-  </si>
-  <si>
-    <t>actions</t>
-  </si>
-  <si>
     <t>apply_date</t>
   </si>
   <si>
-    <t>posted_sal</t>
-  </si>
-  <si>
-    <t>given_sal</t>
-  </si>
-  <si>
-    <t>interview</t>
-  </si>
-  <si>
     <t>link</t>
   </si>
   <si>
@@ -206,6 +178,30 @@
   </si>
   <si>
     <t>position</t>
+  </si>
+  <si>
+    <t>posted_sal_lb</t>
+  </si>
+  <si>
+    <t>posted_sal_ub</t>
+  </si>
+  <si>
+    <t>estimate_sal_lb</t>
+  </si>
+  <si>
+    <t>estimate_sal_ub</t>
+  </si>
+  <si>
+    <t>start</t>
+  </si>
+  <si>
+    <t>end</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>k</t>
   </si>
 </sst>
 </file>
@@ -255,12 +251,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -576,10 +569,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AFE5892-959D-F94B-B9B4-46E79E09F75E}">
-  <dimension ref="A1:Q18"/>
+  <dimension ref="A1:Q20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3:M12"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -595,368 +589,378 @@
     <col min="9" max="9" width="19.33203125" customWidth="1"/>
     <col min="10" max="10" width="24" customWidth="1"/>
     <col min="11" max="11" width="16.5" customWidth="1"/>
+    <col min="12" max="12" width="15.1640625" customWidth="1"/>
+    <col min="13" max="13" width="16.5" customWidth="1"/>
+    <col min="14" max="14" width="15.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="3" t="s">
+      <c r="F3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="G3" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="H3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K3" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="L3" s="1"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>22</v>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K4" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="H6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H6" s="1" t="s">
-        <v>17</v>
-      </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B7" s="2" t="s">
-        <v>10</v>
+      <c r="B7" t="s">
+        <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D7" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E7" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F7" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="G7" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="H7" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="E9" s="1" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>17</v>
+        <v>52</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>21</v>
+        <v>53</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B10" s="2" t="s">
-        <v>10</v>
+      <c r="B10" t="s">
+        <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D10" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E10" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F10" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="G10" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="H10" t="s">
-        <v>22</v>
+        <v>19</v>
+      </c>
+      <c r="I10" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B13" s="2" t="s">
-        <v>10</v>
+      <c r="B13" t="s">
+        <v>9</v>
       </c>
       <c r="C13" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D13" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E13" t="s">
-        <v>22</v>
-      </c>
-      <c r="F13" t="s">
-        <v>22</v>
-      </c>
-      <c r="G13" t="s">
-        <v>22</v>
-      </c>
-      <c r="H13" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C15" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J15" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E15" s="1" t="s">
+      <c r="K15" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="O15" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="P15" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="G15" s="1" t="s">
+      <c r="Q15" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="H15" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="K15" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="L15" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="M15" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="N15" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="O15" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="P15" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q15" s="1" t="s">
-        <v>42</v>
-      </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B16" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="G16" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="H16" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="I16" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="J16" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="K16" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="L16" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="M16" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="N16" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="O16" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="P16" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q16" s="5" t="s">
-        <v>22</v>
+      <c r="B16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L16" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M16" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="N16" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O16" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="P16" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q16" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C18" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G18" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D18" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E18" s="1" t="s">
+      <c r="H18" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="I18" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G18" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="I18" s="1" t="s">
-        <v>40</v>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>